<commit_message>
Added ElementSort; HTML Formatting fixes
</commit_message>
<xml_diff>
--- a/structuretypes.xlsx
+++ b/structuretypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="777" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="777" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CdI2" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="La2CuO4" sheetId="5" r:id="rId5"/>
     <sheet name="NiAs" sheetId="6" r:id="rId6"/>
     <sheet name="SmSI" sheetId="7" r:id="rId7"/>
+    <sheet name="ThCr2Si2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="181">
   <si>
     <t>Structure</t>
   </si>
@@ -446,6 +447,123 @@
   </si>
   <si>
     <t>CrTe</t>
+  </si>
+  <si>
+    <t>ZrNX</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>ZrNCl</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Sr</t>
+  </si>
+  <si>
+    <t>Ba</t>
+  </si>
+  <si>
+    <t>Ba(FeAs)2</t>
+  </si>
+  <si>
+    <t>X(YAs)2</t>
+  </si>
+  <si>
+    <t>Ba(NiAs)2</t>
+  </si>
+  <si>
+    <t>Ca(CoAs)2</t>
+  </si>
+  <si>
+    <t>Ca(NiAs)2</t>
+  </si>
+  <si>
+    <t>Nd</t>
+  </si>
+  <si>
+    <t>Pm</t>
+  </si>
+  <si>
+    <t>Sm</t>
+  </si>
+  <si>
+    <t>Eu</t>
+  </si>
+  <si>
+    <t>Gd</t>
+  </si>
+  <si>
+    <t>Ce(CoAs)2</t>
+  </si>
+  <si>
+    <t>Ce(NiAs)2</t>
+  </si>
+  <si>
+    <t>Eu(CoAs)2</t>
+  </si>
+  <si>
+    <t>Eu(NiAs)2</t>
+  </si>
+  <si>
+    <t>Gd(NiAs)2</t>
+  </si>
+  <si>
+    <t>La(CoAs)2</t>
+  </si>
+  <si>
+    <t>La(NiAs)2</t>
+  </si>
+  <si>
+    <t>Nd(CoAs)2</t>
+  </si>
+  <si>
+    <t>Nd(NiAs)2</t>
+  </si>
+  <si>
+    <t>Pr(CoAs)2</t>
+  </si>
+  <si>
+    <t>Pr(NiAs)2</t>
+  </si>
+  <si>
+    <t>Sm(NiAs)2</t>
+  </si>
+  <si>
+    <t>Sr(CoAs)2</t>
+  </si>
+  <si>
+    <t>Sr(NiAs)2</t>
+  </si>
+  <si>
+    <t>Dy</t>
+  </si>
+  <si>
+    <t>Tb</t>
+  </si>
+  <si>
+    <t>Ho</t>
+  </si>
+  <si>
+    <t>Er</t>
+  </si>
+  <si>
+    <t>X(YB)2</t>
   </si>
 </sst>
 </file>
@@ -1517,14 +1635,270 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>155</v>
+      </c>
+      <c r="J7" t="s">
+        <v>174</v>
+      </c>
+      <c r="M7" t="s">
+        <v>167</v>
+      </c>
+      <c r="N7" t="s">
+        <v>162</v>
+      </c>
+      <c r="O7" t="s">
+        <v>171</v>
+      </c>
+      <c r="P7" t="s">
+        <v>169</v>
+      </c>
+      <c r="R7" t="s">
+        <v>173</v>
+      </c>
+      <c r="S7" t="s">
+        <v>164</v>
+      </c>
+      <c r="T7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>156</v>
+      </c>
+      <c r="J8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" t="s">
+        <v>154</v>
+      </c>
+      <c r="M8" t="s">
+        <v>168</v>
+      </c>
+      <c r="N8" t="s">
+        <v>163</v>
+      </c>
+      <c r="O8" t="s">
+        <v>172</v>
+      </c>
+      <c r="P8" t="s">
+        <v>170</v>
+      </c>
+      <c r="S8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>